<commit_message>
Parte 3 - aire finalizada
</commit_message>
<xml_diff>
--- a/Interferometria/Datos_23_sept.xlsx
+++ b/Interferometria/Datos_23_sept.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaalvarezlopez/Documents/Universidad/Noveno Semestre/Laboratorio Intermedio/Laboratorios/Interferometría/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaalvarezlopez/Documents/Universidad/Noveno Semestre/Laboratorio Intermedio/Laboratorios/Interferometria/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B81AF3-32CB-0D42-89EC-593A6F56DDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0BEAACB-552A-7A4C-8569-9347EA907C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="3" xr2:uid="{24852B43-6C13-CC4F-BB83-8CFD8895B4C1}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Los de 800" sheetId="4" r:id="rId2"/>
     <sheet name="Vidrio" sheetId="2" r:id="rId3"/>
     <sheet name="Aire" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>micro m</t>
   </si>
@@ -105,6 +106,27 @@
   <si>
     <t>dn/dP</t>
   </si>
+  <si>
+    <t>dn</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Hpa</t>
+  </si>
+  <si>
+    <t>cm Hg</t>
+  </si>
+  <si>
+    <t>P_atm</t>
+  </si>
+  <si>
+    <t>dP</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,17 +172,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1199,6 +1233,383 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Aire!$A$3:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Aire!$G$3:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.0001825999747771</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.000172049974777</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0001614999747772</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0001509499747772</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0001403999747771</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0001298499747771</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0001192999747772</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0000981999747771</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0000876499747771</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000770999747772</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000665499747772</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0000559999747771</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0000454499747771</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0000348999747772</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0000243499747772</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA6D-7742-9317-CAD8CB317E22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="801564415"/>
+        <c:axId val="801484159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="801564415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801484159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="801484159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801564415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1279,6 +1690,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1796,6 +2247,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2379,6 +3346,47 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>237377</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>547230</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>164767</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B381007-6CFF-8B44-8799-3FDC83A40105}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2695,7 +3703,7 @@
   <dimension ref="B1:M37"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2746,7 +3754,7 @@
         <v>2</v>
       </c>
       <c r="H3">
-        <f>2*E3/G3</f>
+        <f t="shared" ref="H3:H18" si="0">2*E3/G3</f>
         <v>1</v>
       </c>
       <c r="L3">
@@ -2774,7 +3782,7 @@
         <v>6</v>
       </c>
       <c r="H4">
-        <f>2*E4/G4</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="L4">
@@ -2802,7 +3810,7 @@
         <v>12</v>
       </c>
       <c r="H5">
-        <f>2*E5/G5</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="L5">
@@ -2830,7 +3838,7 @@
         <v>14</v>
       </c>
       <c r="H6">
-        <f>2*E6/G6</f>
+        <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -2852,7 +3860,7 @@
         <v>16</v>
       </c>
       <c r="H7">
-        <f>2*E7/G7</f>
+        <f t="shared" si="0"/>
         <v>0.625</v>
       </c>
     </row>
@@ -2874,7 +3882,7 @@
         <v>19</v>
       </c>
       <c r="H8">
-        <f>2*E8/G8</f>
+        <f t="shared" si="0"/>
         <v>0.63157894736842102</v>
       </c>
     </row>
@@ -2890,7 +3898,7 @@
         <v>22</v>
       </c>
       <c r="H9">
-        <f>2*E9/G9</f>
+        <f t="shared" si="0"/>
         <v>0.63636363636363635</v>
       </c>
     </row>
@@ -2906,7 +3914,7 @@
         <v>25</v>
       </c>
       <c r="H10">
-        <f>2*E10/G10</f>
+        <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
     </row>
@@ -2922,7 +3930,7 @@
         <v>28</v>
       </c>
       <c r="H11">
-        <f>2*E11/G11</f>
+        <f t="shared" si="0"/>
         <v>0.6428571428571429</v>
       </c>
     </row>
@@ -2938,7 +3946,7 @@
         <v>31</v>
       </c>
       <c r="H12">
-        <f>2*E12/G12</f>
+        <f t="shared" si="0"/>
         <v>0.64516129032258063</v>
       </c>
     </row>
@@ -2954,7 +3962,7 @@
         <v>34</v>
       </c>
       <c r="H13">
-        <f>2*E13/G13</f>
+        <f t="shared" si="0"/>
         <v>0.6470588235294118</v>
       </c>
     </row>
@@ -2970,7 +3978,7 @@
         <v>37</v>
       </c>
       <c r="H14">
-        <f>2*E14/G14</f>
+        <f t="shared" si="0"/>
         <v>0.64864864864864868</v>
       </c>
     </row>
@@ -2986,7 +3994,7 @@
         <v>40</v>
       </c>
       <c r="H15">
-        <f>2*E15/G15</f>
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
     </row>
@@ -3002,7 +4010,7 @@
         <v>42</v>
       </c>
       <c r="H16">
-        <f>2*E16/G16</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -3018,7 +4026,7 @@
         <v>45</v>
       </c>
       <c r="H17">
-        <f>2*E17/G17</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -3034,7 +4042,7 @@
         <v>48</v>
       </c>
       <c r="H18">
-        <f>2*E18/G18</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -3107,7 +4115,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <f>2*C3/E3</f>
+        <f t="shared" ref="F3:F18" si="0">2*C3/E3</f>
         <v>1</v>
       </c>
     </row>
@@ -3120,7 +4128,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <f>2*C4/E4</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3136,7 +4144,7 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <f>2*C5/E5</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
@@ -3152,7 +4160,7 @@
         <v>7</v>
       </c>
       <c r="F6">
-        <f>2*C6/E6</f>
+        <f t="shared" si="0"/>
         <v>1.1428571428571428</v>
       </c>
     </row>
@@ -3165,7 +4173,7 @@
         <v>7</v>
       </c>
       <c r="F7">
-        <f>2*C7/E7</f>
+        <f t="shared" si="0"/>
         <v>1.4285714285714286</v>
       </c>
     </row>
@@ -3181,7 +4189,7 @@
         <v>12</v>
       </c>
       <c r="F8">
-        <f>2*C8/E8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3197,7 +4205,7 @@
         <v>15</v>
       </c>
       <c r="F9">
-        <f>2*C9/E9</f>
+        <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
     </row>
@@ -3213,7 +4221,7 @@
         <v>18</v>
       </c>
       <c r="F10">
-        <f>2*C10/E10</f>
+        <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
@@ -3226,7 +4234,7 @@
         <v>18</v>
       </c>
       <c r="F11">
-        <f>2*C11/E11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3242,7 +4250,7 @@
         <v>22</v>
       </c>
       <c r="F12">
-        <f>2*C12/E12</f>
+        <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
     </row>
@@ -3255,7 +4263,7 @@
         <v>22</v>
       </c>
       <c r="F13">
-        <f>2*C13/E13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3268,7 +4276,7 @@
         <v>22</v>
       </c>
       <c r="F14">
-        <f>2*C14/E14</f>
+        <f t="shared" si="0"/>
         <v>1.0909090909090908</v>
       </c>
     </row>
@@ -3284,7 +4292,7 @@
         <v>29</v>
       </c>
       <c r="F15">
-        <f>2*C15/E15</f>
+        <f t="shared" si="0"/>
         <v>0.89655172413793105</v>
       </c>
     </row>
@@ -3300,7 +4308,7 @@
         <v>31</v>
       </c>
       <c r="F16">
-        <f>2*C16/E16</f>
+        <f t="shared" si="0"/>
         <v>0.90322580645161288</v>
       </c>
     </row>
@@ -3313,7 +4321,7 @@
         <v>31</v>
       </c>
       <c r="F17">
-        <f>2*C17/E17</f>
+        <f t="shared" si="0"/>
         <v>0.967741935483871</v>
       </c>
     </row>
@@ -3329,7 +4337,7 @@
         <v>36</v>
       </c>
       <c r="F18">
-        <f>2*C18/E18</f>
+        <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
@@ -3344,7 +4352,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3412,7 +4420,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E19" si="1">(2*$H$2 - D3*$H$3)*(1- COS(RADIANS(B3)))/((2*$H$2)*(1-COS(RADIANS(B3))) - D3*$H$3)</f>
+        <f>(2*$H$2 - D3*$H$3)*(1- COS(RADIANS(B3)))/((2*$H$2)*(1-COS(RADIANS(B3))) - D3*$H$3)</f>
         <v>1.501194037333353</v>
       </c>
       <c r="G3" t="s">
@@ -3438,7 +4446,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D4*$H$3)*(1- COS(RADIANS(B4)))/((2*$H$2)*(1-COS(RADIANS(B4))) - D4*$H$3)</f>
         <v>1.457303683719918</v>
       </c>
     </row>
@@ -3458,7 +4466,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D5*$H$3)*(1- COS(RADIANS(B5)))/((2*$H$2)*(1-COS(RADIANS(B5))) - D5*$H$3)</f>
         <v>1.4853282162226011</v>
       </c>
     </row>
@@ -3478,7 +4486,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D6*$H$3)*(1- COS(RADIANS(B6)))/((2*$H$2)*(1-COS(RADIANS(B6))) - D6*$H$3)</f>
         <v>1.4025002869037881</v>
       </c>
     </row>
@@ -3498,7 +4506,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D7*$H$3)*(1- COS(RADIANS(B7)))/((2*$H$2)*(1-COS(RADIANS(B7))) - D7*$H$3)</f>
         <v>1.3803108031333724</v>
       </c>
     </row>
@@ -3518,7 +4526,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D8*$H$3)*(1- COS(RADIANS(B8)))/((2*$H$2)*(1-COS(RADIANS(B8))) - D8*$H$3)</f>
         <v>1.3586935158055637</v>
       </c>
     </row>
@@ -3538,7 +4546,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D9*$H$3)*(1- COS(RADIANS(B9)))/((2*$H$2)*(1-COS(RADIANS(B9))) - D9*$H$3)</f>
         <v>1.3922447149986636</v>
       </c>
     </row>
@@ -3558,7 +4566,7 @@
         <v>41</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D10*$H$3)*(1- COS(RADIANS(B10)))/((2*$H$2)*(1-COS(RADIANS(B10))) - D10*$H$3)</f>
         <v>1.3600174873300093</v>
       </c>
     </row>
@@ -3578,7 +4586,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D11*$H$3)*(1- COS(RADIANS(B11)))/((2*$H$2)*(1-COS(RADIANS(B11))) - D11*$H$3)</f>
         <v>1.3794162207296283</v>
       </c>
     </row>
@@ -3598,7 +4606,7 @@
         <v>51</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D12*$H$3)*(1- COS(RADIANS(B12)))/((2*$H$2)*(1-COS(RADIANS(B12))) - D12*$H$3)</f>
         <v>1.3697234666406746</v>
       </c>
     </row>
@@ -3618,7 +4626,7 @@
         <v>56</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D13*$H$3)*(1- COS(RADIANS(B13)))/((2*$H$2)*(1-COS(RADIANS(B13))) - D13*$H$3)</f>
         <v>1.3820220296829817</v>
       </c>
     </row>
@@ -3638,7 +4646,7 @@
         <v>61</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D14*$H$3)*(1- COS(RADIANS(B14)))/((2*$H$2)*(1-COS(RADIANS(B14))) - D14*$H$3)</f>
         <v>1.3917234246681383</v>
       </c>
     </row>
@@ -3658,7 +4666,7 @@
         <v>66</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D15*$H$3)*(1- COS(RADIANS(B15)))/((2*$H$2)*(1-COS(RADIANS(B15))) - D15*$H$3)</f>
         <v>1.3874391656875751</v>
       </c>
     </row>
@@ -3678,7 +4686,7 @@
         <v>72</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D16*$H$3)*(1- COS(RADIANS(B16)))/((2*$H$2)*(1-COS(RADIANS(B16))) - D16*$H$3)</f>
         <v>1.4008674259607461</v>
       </c>
     </row>
@@ -3698,7 +4706,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D17*$H$3)*(1- COS(RADIANS(B17)))/((2*$H$2)*(1-COS(RADIANS(B17))) - D17*$H$3)</f>
         <v>1.4005067772940003</v>
       </c>
     </row>
@@ -3718,7 +4726,7 @@
         <v>83</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D18*$H$3)*(1- COS(RADIANS(B18)))/((2*$H$2)*(1-COS(RADIANS(B18))) - D18*$H$3)</f>
         <v>1.4253814535931528</v>
       </c>
     </row>
@@ -3738,7 +4746,7 @@
         <v>88</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
+        <f>(2*$H$2 - D19*$H$3)*(1- COS(RADIANS(B19)))/((2*$H$2)*(1-COS(RADIANS(B19))) - D19*$H$3)</f>
         <v>1.4257236258405037</v>
       </c>
     </row>
@@ -3917,20 +4925,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A800733E-6DDA-9E49-BF38-469F6286CDEB}">
-  <dimension ref="B2:J17"/>
+  <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -3943,6 +4955,12 @@
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
@@ -3950,7 +4968,11 @@
         <v>633</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>$J$5-B3</f>
+        <v>50</v>
+      </c>
       <c r="B3" s="1">
         <v>6</v>
       </c>
@@ -3965,6 +4987,14 @@
         <f>D3*$J$2/(2*$J$3*B3)</f>
         <v>1.7583333333333334E-6</v>
       </c>
+      <c r="F3">
+        <f>E3*B3</f>
+        <v>1.0550000000000001E-5</v>
+      </c>
+      <c r="G3">
+        <f>$E$37-F3</f>
+        <v>1.0001825999747771</v>
+      </c>
       <c r="I3" t="s">
         <v>5</v>
       </c>
@@ -3973,7 +5003,11 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A17" si="0">$J$5-B4</f>
+        <v>46</v>
+      </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
@@ -3985,11 +5019,32 @@
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E17" si="0">D4*$J$2/(2*$J$3*B4)</f>
+        <f t="shared" ref="E4:E17" si="1">D4*$J$2/(2*$J$3*B4)</f>
         <v>2.1100000000000001E-6</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" ref="F4:F17" si="2">E4*B4</f>
+        <v>2.1100000000000001E-5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G17" si="3">$E$37-F4</f>
+        <v>1.000172049974777</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>751.5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
       <c r="B5" s="1">
         <v>14</v>
       </c>
@@ -4001,11 +5056,33 @@
         <v>3</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2607142857142858E-6</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>3.1650000000000004E-5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1.0001614999747772</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <f>ROUND(J4*0.075,0)</f>
+        <v>56</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="B6" s="1">
         <v>16</v>
       </c>
@@ -4017,11 +5094,23 @@
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f>D6*$J$2/(2*$J$3*B6)</f>
         <v>2.6375000000000002E-6</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>4.2200000000000003E-5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>1.0001509499747772</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="B7" s="1">
         <v>20</v>
       </c>
@@ -4033,11 +5122,23 @@
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6375000000000002E-6</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>5.2750000000000001E-5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1.0001403999747771</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="B8" s="1">
         <v>22</v>
       </c>
@@ -4049,11 +5150,23 @@
         <v>6</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8772727272727275E-6</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>6.3300000000000007E-5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>1.0001298499747771</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="B9" s="1">
         <v>26</v>
       </c>
@@ -4065,11 +5178,23 @@
         <v>7</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8403846153846154E-6</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>7.3850000000000006E-5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>1.0001192999747772</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="B10" s="1">
         <v>32</v>
       </c>
@@ -4081,11 +5206,23 @@
         <v>9</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9671875000000001E-6</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>9.4950000000000004E-5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1.0000981999747771</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
       <c r="B11" s="1">
         <v>34</v>
       </c>
@@ -4097,11 +5234,23 @@
         <v>10</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.102941176470588E-6</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1.0549999999999999E-4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>1.0000876499747771</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="B12" s="1">
         <v>38</v>
       </c>
@@ -4113,11 +5262,23 @@
         <v>11</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0539473684210524E-6</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1.1604999999999999E-4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>1.0000770999747772</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="B13" s="1">
         <v>42</v>
       </c>
@@ -4129,11 +5290,23 @@
         <v>12</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0142857142857141E-6</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1.2659999999999999E-4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>1.0000665499747772</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="B14" s="1">
         <v>44</v>
       </c>
@@ -4145,11 +5318,23 @@
         <v>13</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1170454545454544E-6</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>1.3715E-4</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>1.0000559999747771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="B15" s="1">
         <v>46</v>
       </c>
@@ -4161,11 +5346,23 @@
         <v>14</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2108695652173915E-6</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>1.4770000000000001E-4</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>1.0000454499747771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="B16" s="3">
         <v>50</v>
       </c>
@@ -4177,11 +5374,23 @@
         <v>15</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1650000000000002E-6</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>1.5825E-4</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>1.0000348999747772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="B17" s="3">
         <v>52</v>
       </c>
@@ -4193,8 +5402,175 @@
         <v>16</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2461538461538462E-6</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>1.6880000000000001E-4</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>1.0000243499747772</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E35" cm="1">
+        <f t="array" ref="E35:F35">LINEST(F3:F17,A3:A17)</f>
+        <v>-3.4491066924499751E-6</v>
+      </c>
+      <c r="F35">
+        <v>1.7924355977803934E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <f>-E35*J5 + 1</f>
+        <v>1.0001931499747772</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB8139F-7657-584A-8473-9636BB73B302}">
+  <dimension ref="B3:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1.0001825999747771</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1.000172049974777</v>
+      </c>
+      <c r="C5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1.0001614999747772</v>
+      </c>
+      <c r="C6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>1.0001509499747772</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>1.0001403999747771</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>1.0001298499747771</v>
+      </c>
+      <c r="C9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>1.0001192999747772</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>1.0000981999747771</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>1.0000876499747771</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1.0000770999747772</v>
+      </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>1.0000665499747772</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>1.0000559999747771</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>1.0000454499747771</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>1.0000348999747772</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>1.0000243499747772</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>